<commit_message>
Updated Summarize macra and produced eb and wb tracks
</commit_message>
<xml_diff>
--- a/Route Summary.xlsx
+++ b/Route Summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CP Dir1" sheetId="1" r:id="rId1"/>
@@ -526,8 +526,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,18 +1960,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:G46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1986,7 +1988,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2008,8 +2010,16 @@
       <c r="G2">
         <v>54.03</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="2">
+        <f>(D2/60+C2)/60+B2</f>
+        <v>43.52279166666667</v>
+      </c>
+      <c r="I2" s="2">
+        <f>-((G2/60+F2)/60+E2)</f>
+        <v>-79.681674999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -2031,8 +2041,16 @@
       <c r="G3">
         <v>3.18</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H46" si="0">(D3/60+C3)/60+B3</f>
+        <v>43.520377777777774</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I46" si="1">-((G3/60+F3)/60+E3)</f>
+        <v>-79.684216666666671</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -2054,8 +2072,16 @@
       <c r="G4">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="2">
+        <f t="shared" si="0"/>
+        <v>43.517747222222219</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.687083333333334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -2077,8 +2103,16 @@
       <c r="G5">
         <v>22.04</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>43.515547222222224</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.689455555555554</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2100,8 +2134,16 @@
       <c r="G6">
         <v>30.42</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>43.513402777777777</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.691783333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2123,8 +2165,16 @@
       <c r="G7">
         <v>34.57</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>43.51230833333333</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.692936111111109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -2146,8 +2196,16 @@
       <c r="G8">
         <v>40.71</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>43.510755555555555</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.694641666666669</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -2169,8 +2227,16 @@
       <c r="G9">
         <v>46.79</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>43.509188888888886</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.696330555555562</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -2192,8 +2258,16 @@
       <c r="G10">
         <v>50.59</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>43.50823888888889</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.697386111111115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -2215,8 +2289,16 @@
       <c r="G11">
         <v>14.29</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>43.502163888888887</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.703969444444439</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2238,8 +2320,16 @@
       <c r="G12">
         <v>30.87</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>43.497969444444443</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.708574999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2261,8 +2351,16 @@
       <c r="G13">
         <v>47.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>43.493694444444444</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.713277777777776</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2284,8 +2382,16 @@
       <c r="G14">
         <v>59.47</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>43.490711111111111</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.716519444444444</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -2307,8 +2413,16 @@
       <c r="G15">
         <v>10.58</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>43.487877777777776</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.71960555555556</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2330,8 +2444,16 @@
       <c r="G16">
         <v>26.19</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
+        <v>43.484016666666669</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.723941666666661</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2353,8 +2475,16 @@
       <c r="G17">
         <v>37.44</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2">
+        <f t="shared" si="0"/>
+        <v>43.481163888888887</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.727066666666673</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2376,8 +2506,16 @@
       <c r="G18">
         <v>45.29</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="2">
+        <f t="shared" si="0"/>
+        <v>43.479188888888892</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.729247222222227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -2399,8 +2537,16 @@
       <c r="G19">
         <v>4.43</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="2">
+        <f t="shared" si="0"/>
+        <v>43.474261111111112</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.734563888888886</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2422,8 +2568,16 @@
       <c r="G20">
         <v>23.38</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="2">
+        <f t="shared" si="0"/>
+        <v>43.469494444444443</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.739827777777776</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2445,8 +2599,16 @@
       <c r="G21">
         <v>42.22</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="2">
+        <f t="shared" si="0"/>
+        <v>43.464713888888888</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.745061111111113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2468,8 +2630,16 @@
       <c r="G22">
         <v>57.27</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="2">
+        <f t="shared" si="0"/>
+        <v>43.461041666666667</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.749241666666663</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -2491,8 +2661,16 @@
       <c r="G23">
         <v>14.3</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="2">
+        <f t="shared" si="0"/>
+        <v>43.45666111111111</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.753972222222217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2514,8 +2692,16 @@
       <c r="G24">
         <v>26.13</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="2">
+        <f t="shared" si="0"/>
+        <v>43.453622222222222</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.75725833333334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2537,8 +2723,16 @@
       <c r="G25">
         <v>39.17</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="2">
+        <f t="shared" si="0"/>
+        <v>43.450311111111112</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.760880555555559</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -2560,8 +2754,16 @@
       <c r="G26">
         <v>4.92</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="2">
+        <f t="shared" si="0"/>
+        <v>43.443647222222225</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.768033333333335</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -2583,8 +2785,16 @@
       <c r="G27">
         <v>34.96</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="2">
+        <f t="shared" si="0"/>
+        <v>43.435655555555556</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.776377777777782</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -2606,8 +2816,16 @@
       <c r="G28">
         <v>38.74</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="2">
+        <f t="shared" si="0"/>
+        <v>34.434697222222219</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.777427777777774</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -2629,8 +2847,16 @@
       <c r="G29">
         <v>45.74</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="2">
+        <f t="shared" si="0"/>
+        <v>43.432977777777779</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.779372222222221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -2652,8 +2878,16 @@
       <c r="G30">
         <v>59.74</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="2">
+        <f t="shared" si="0"/>
+        <v>43.429216666666669</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.783261111111116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -2675,8 +2909,16 @@
       <c r="G31">
         <v>31.42</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="2">
+        <f t="shared" si="0"/>
+        <v>43.421063888888888</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.79206111111111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -2698,8 +2940,16 @@
       <c r="G32">
         <v>7.43</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="2">
+        <f t="shared" si="0"/>
+        <v>43.412061111111115</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.802063888888895</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -2721,8 +2971,16 @@
       <c r="G33">
         <v>28.64</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="2">
+        <f t="shared" si="0"/>
+        <v>43.406605555555558</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.807955555555552</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -2744,8 +3002,16 @@
       <c r="G34">
         <v>51.18</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="2">
+        <f t="shared" si="0"/>
+        <v>43.400799999999997</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.814216666666667</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2767,8 +3033,16 @@
       <c r="G35">
         <v>2.85</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="2">
+        <f t="shared" si="0"/>
+        <v>43.397827777777778</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.817458333333335</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -2790,8 +3064,16 @@
       <c r="G36">
         <v>13.98</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="2">
+        <f t="shared" si="0"/>
+        <v>43.395030555555557</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.820549999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -2813,8 +3095,16 @@
       <c r="G37">
         <v>25.75</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="2">
+        <f t="shared" si="0"/>
+        <v>43.39212777777778</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.823819444444439</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2836,8 +3126,16 @@
       <c r="G38">
         <v>37.89</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="2">
+        <f t="shared" si="0"/>
+        <v>43.389208333333336</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.827191666666664</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2859,8 +3157,16 @@
       <c r="G39">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="2">
+        <f t="shared" si="0"/>
+        <v>43.383652777777776</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.833355555555556</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -2882,8 +3188,16 @@
       <c r="G40">
         <v>5.15</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="2">
+        <f t="shared" si="0"/>
+        <v>43.382333333333335</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.834763888888887</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -2905,8 +3219,16 @@
       <c r="G41">
         <v>12.38</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="2">
+        <f t="shared" si="0"/>
+        <v>43.380447222222223</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.836772222222223</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -2928,8 +3250,16 @@
       <c r="G42">
         <v>22.98</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="2">
+        <f t="shared" si="0"/>
+        <v>43.377802777777781</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.839716666666661</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -2951,8 +3281,16 @@
       <c r="G43">
         <v>40.380000000000003</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="2">
+        <f t="shared" si="0"/>
+        <v>43.373583333333336</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.844549999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -2974,8 +3312,16 @@
       <c r="G44">
         <v>57.74</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="2">
+        <f t="shared" si="0"/>
+        <v>43.369327777777777</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.849372222222229</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -2997,8 +3343,16 @@
       <c r="G45">
         <v>20.67</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="2">
+        <f t="shared" si="0"/>
+        <v>43.363758333333337</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.85574166666666</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -3019,6 +3373,14 @@
       </c>
       <c r="G46">
         <v>5.12</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="0"/>
+        <v>43.352802777777775</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="1"/>
+        <v>-79.868088888888892</v>
       </c>
     </row>
   </sheetData>

</xml_diff>